<commit_message>
- support any SQL, even those with custom SQL syntax - added more test cases
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/org/nexial/core/variable/ExpressionProcessorTest10.xlsx
+++ b/src/test/resources/org/nexial/core/variable/ExpressionProcessorTest10.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10305"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/com/ep/qa/sentry/variable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/org/nexial/core/variable/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78BD450-69A4-4F49-8B0D-6BB584371482}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21160" windowWidth="38400" windowHeight="21160" activeTab="4"/>
+    <workbookView xWindow="9140" yWindow="-20560" windowWidth="33600" windowHeight="10280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ipsSC1" sheetId="1" r:id="rId1"/>
-    <sheet name="ipsTC1" sheetId="2" r:id="rId2"/>
-    <sheet name="Clients" sheetId="6" r:id="rId3"/>
-    <sheet name="Test Case Covg" sheetId="8" r:id="rId4"/>
+    <sheet name="sc1" sheetId="1" r:id="rId1"/>
+    <sheet name="tc17" sheetId="2" r:id="rId2"/>
+    <sheet name="list45" sheetId="6" r:id="rId3"/>
+    <sheet name="rccTo_2355" sheetId="8" r:id="rId4"/>
     <sheet name="transposed" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ipsSC1!$A$2:$AJ$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ipsTC1!$A$1:$R$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'sc1'!$A$2:$AJ$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'tc17'!$A$1:$R$1</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="157">
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>tax id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="154">
   <si>
     <t>name</t>
   </si>
@@ -127,9 +122,6 @@
     <t>tax waiver</t>
   </si>
   <si>
-    <t>invoice no</t>
-  </si>
-  <si>
     <t>work date</t>
   </si>
   <si>
@@ -163,9 +155,6 @@
     <t>class code</t>
   </si>
   <si>
-    <t>Laura's notes</t>
-  </si>
-  <si>
     <t>fid</t>
   </si>
   <si>
@@ -286,9 +275,6 @@
     <t>NJ</t>
   </si>
   <si>
-    <t>Corps only</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
@@ -388,9 +374,6 @@
     <t>a-checks???</t>
   </si>
   <si>
-    <t>invoice</t>
-  </si>
-  <si>
     <t>fla/</t>
   </si>
   <si>
@@ -506,12 +489,21 @@
   </si>
   <si>
     <t>Hello there!</t>
+  </si>
+  <si>
+    <t>number1</t>
+  </si>
+  <si>
+    <t>numbers3</t>
+  </si>
+  <si>
+    <t>numbers2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -612,6 +604,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -903,12 +898,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BD6"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -924,11 +917,9 @@
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>83</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="AO1" s="7"/>
       <c r="AP1" s="7"/>
       <c r="AQ1" s="7"/>
       <c r="AR1" s="7"/>
@@ -939,9 +930,7 @@
       <c r="AW1" s="7"/>
       <c r="AX1" s="7"/>
       <c r="AY1" s="7"/>
-      <c r="AZ1" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="AZ1" s="6"/>
       <c r="BA1" s="6"/>
       <c r="BB1" s="6"/>
       <c r="BC1" s="6"/>
@@ -949,160 +938,160 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
       <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="W2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AA2" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>21</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>22</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG2" t="s">
         <v>23</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AH2" t="s">
         <v>24</v>
       </c>
-      <c r="AF2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AI2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AK2" t="s">
         <v>27</v>
       </c>
-      <c r="AJ2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>29</v>
-      </c>
       <c r="AL2" s="3" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="AM2" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="AN2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AO2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AP2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AQ2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AW2" t="s">
         <v>84</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AX2" t="s">
         <v>85</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AY2" t="s">
         <v>86</v>
       </c>
-      <c r="AT2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>89</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>91</v>
-      </c>
       <c r="AZ2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.2">
@@ -1113,64 +1102,64 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>2300001</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L3">
         <v>91504</v>
       </c>
       <c r="M3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W3">
         <v>17</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AA3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AD3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AF3">
         <v>3</v>
@@ -1182,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.2">
@@ -1193,61 +1182,61 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H4">
         <v>1100056</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L4">
         <v>91504</v>
       </c>
       <c r="M4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W4">
         <v>17</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AD4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AF4">
         <v>3</v>
@@ -1259,19 +1248,19 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="AK4">
         <v>3</v>
       </c>
       <c r="AL4" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="AM4" s="5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="AN4" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.2">
@@ -1282,40 +1271,40 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E5">
         <v>652521225</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H5">
         <v>2901001</v>
       </c>
       <c r="I5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L5">
         <v>91504</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -1324,31 +1313,31 @@
         <v>5</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W5">
         <v>17</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AB5">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="AD5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AE5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="AF5">
         <v>3</v>
@@ -1360,40 +1349,40 @@
         <v>3</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="AO5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AP5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AQ5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AR5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AS5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AT5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AU5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AV5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AW5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AX5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AY5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.2">
@@ -1404,64 +1393,64 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H6">
         <v>9400001</v>
       </c>
       <c r="I6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="L6">
         <v>91504</v>
       </c>
       <c r="M6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="N6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="W6">
         <v>17</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="AA6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AD6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="AF6">
         <v>3</v>
@@ -1473,20 +1462,22 @@
         <v>1</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AJ2"/>
+  <autoFilter ref="A2:AJ2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1499,58 +1490,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>38</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -1561,25 +1552,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L2">
         <v>5</v>
@@ -1602,25 +1593,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L3">
         <v>5</v>
@@ -1643,25 +1634,25 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L4">
         <v>5</v>
@@ -1684,25 +1675,25 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L5">
         <v>5</v>
@@ -1722,25 +1713,25 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L6">
         <v>5</v>
@@ -1763,19 +1754,19 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1798,19 +1789,19 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1833,19 +1824,19 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1868,19 +1859,19 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1903,25 +1894,25 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L11">
         <v>5</v>
@@ -1941,19 +1932,19 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1973,19 +1964,19 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -2005,19 +1996,19 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2037,19 +2028,19 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -2069,25 +2060,25 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L16">
         <v>5</v>
@@ -2107,19 +2098,19 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -2139,19 +2130,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2171,28 +2162,28 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L19">
         <v>5</v>
@@ -2212,25 +2203,25 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="O20">
         <v>861</v>
@@ -2247,25 +2238,25 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="O21">
         <v>110</v>
@@ -2285,25 +2276,25 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="O22">
         <v>350</v>
@@ -2323,25 +2314,25 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="O23">
         <v>360</v>
@@ -2361,62 +2352,60 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R1"/>
+  <autoFilter ref="A1:R1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2427,10 +2416,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2441,10 +2430,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2455,10 +2444,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2469,10 +2458,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2483,16 +2472,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2503,10 +2492,10 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E7">
         <v>47</v>
@@ -2520,10 +2509,10 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2534,10 +2523,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2548,10 +2537,10 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2562,10 +2551,10 @@
         <v>2000</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -2579,10 +2568,10 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2593,33 +2582,33 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2628,11 +2617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView zoomScale="134" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2646,108 +2635,108 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="G2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="P2" t="s">
+        <v>121</v>
+      </c>
+      <c r="V2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="42" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="P2" t="s">
-        <v>127</v>
-      </c>
-      <c r="V2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="N3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z3" s="8" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="40" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="AC3" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -2758,19 +2747,19 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -2781,19 +2770,19 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -2804,19 +2793,19 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -2827,19 +2816,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -2850,16 +2839,16 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -2870,16 +2859,16 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -2890,16 +2879,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -2910,16 +2899,16 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2929,18 +2918,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="16:16" x14ac:dyDescent="0.2">
       <c r="P4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>